<commit_message>
change fields / remove unused place field
</commit_message>
<xml_diff>
--- a/ospp-application/src/main/resources/devdata/lecturers.xlsx
+++ b/ospp-application/src/main/resources/devdata/lecturers.xlsx
@@ -1,72 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peer\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882BC8EB-D72F-4782-B53E-7669A222107C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileSharing readOnlyRecommended="0" userName="p"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="38640" windowHeight="21240" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr/>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:revision xmlns:pm="smNativeData" day="1593875898" val="976" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1593875898" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1593875898" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1593875898"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>tc={2A1E609B-5249-4D08-B548-F3C7C60441AC}</author>
-    <author>tc={0E2F502E-311A-4D81-9115-93705B70C95D}</author>
-    <author>tc={511EB7D9-C334-404E-82D3-AF6388B14F2E}</author>
-    <author>tc={D6A8E29B-FDC6-4920-8EFE-04825474B544}</author>
-    <author>tc={55035905-0A00-4588-99BC-9E1F5B6F3589}</author>
+    <author>Unknown</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{2A1E609B-5249-4D08-B548-F3C7C60441AC}">
+    <comment ref="B1" authorId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Vorname des Dozenten/Experten</t>
+        </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{0E2F502E-311A-4D81-9115-93705B70C95D}">
+    <comment ref="C1" authorId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Nachname des dozenten/experten</t>
+        </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{511EB7D9-C334-404E-82D3-AF6388B14F2E}">
+    <comment ref="D1" authorId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Kürzel des dozenten. Muss mit dem Dozentenkürzel bei den Präsentationen übereinstimmen.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{D6A8E29B-FDC6-4920-8EFE-04825474B544}">
+    <comment ref="E1" authorId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Email des Dozenten/Experten.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{55035905-0A00-4588-99BC-9E1F5B6F3589}">
+    <comment ref="A1" authorId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     ID des Dozenten/Experten. Muss bei 0 beginnen und aufsteigen. Eine ID darf nicht doppelt vergeben werden.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -76,19 +85,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="531">
   <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>initials</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>id</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Vorname</t>
+  </si>
+  <si>
+    <t>Nachname</t>
+  </si>
+  <si>
+    <t>Kürzel LP</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>Urs</t>
@@ -103,7 +115,7 @@
     <t>urs.abaecherli@edubs.ch</t>
   </si>
   <si>
-    <t>0</t>
+    <t>1</t>
   </si>
   <si>
     <t>Angelo</t>
@@ -118,7 +130,7 @@
     <t>angelo.baltermia@edubs.ch</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
   <si>
     <t>Andreas</t>
@@ -133,7 +145,7 @@
     <t>andreas.baeumler@edubs.ch</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
   <si>
     <t>Karin</t>
@@ -148,7 +160,7 @@
     <t>karin.barth@edubs.ch</t>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
   </si>
   <si>
     <t>Nicole</t>
@@ -163,7 +175,7 @@
     <t>nicole.beer@edubs.ch</t>
   </si>
   <si>
-    <t>4</t>
+    <t>5</t>
   </si>
   <si>
     <t>Salome</t>
@@ -178,7 +190,7 @@
     <t>salome.beaneisenhut@edubs.ch</t>
   </si>
   <si>
-    <t>5</t>
+    <t>6</t>
   </si>
   <si>
     <t>Martin</t>
@@ -193,7 +205,7 @@
     <t>martin.birchler@edubs.ch</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>Valerie</t>
@@ -208,7 +220,7 @@
     <t>valerie.bosshard@edubs.ch</t>
   </si>
   <si>
-    <t>7</t>
+    <t>8</t>
   </si>
   <si>
     <t>Andrea</t>
@@ -223,7 +235,7 @@
     <t>andrea.brand@edubs.ch</t>
   </si>
   <si>
-    <t>8</t>
+    <t>9</t>
   </si>
   <si>
     <t>Robin</t>
@@ -238,7 +250,7 @@
     <t>robin.bruederlin1@edubs.ch</t>
   </si>
   <si>
-    <t>9</t>
+    <t>10</t>
   </si>
   <si>
     <t>Dorothee</t>
@@ -253,7 +265,7 @@
     <t>dorothee.caan@edubs.ch</t>
   </si>
   <si>
-    <t>10</t>
+    <t>11</t>
   </si>
   <si>
     <t>Valentina</t>
@@ -268,7 +280,7 @@
     <t>valentina.dicesare@edubs.ch</t>
   </si>
   <si>
-    <t>11</t>
+    <t>12</t>
   </si>
   <si>
     <t>Tuba</t>
@@ -283,7 +295,7 @@
     <t>tuba.demirbas@gmx.ch</t>
   </si>
   <si>
-    <t>12</t>
+    <t>13</t>
   </si>
   <si>
     <t>Letizia</t>
@@ -298,7 +310,7 @@
     <t>letizia.dipner@edubs.ch</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>Viola</t>
@@ -313,7 +325,7 @@
     <t>viola.ehm@edubs.ch</t>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
   <si>
     <t>Tobias</t>
@@ -328,7 +340,7 @@
     <t>tobias.erhardt@edubs.ch</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
   <si>
     <t>Béla</t>
@@ -343,7 +355,7 @@
     <t>bela.feher@edubs.ch</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
   <si>
     <t>Esther</t>
@@ -358,7 +370,7 @@
     <t>esther.fritzius@edubs.ch</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
   <si>
     <t>Sara</t>
@@ -373,7 +385,7 @@
     <t>sara.fuschetto@edubs.ch</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>Doris</t>
@@ -388,7 +400,7 @@
     <t>doris.gabler@edubs.ch</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>Fabienne</t>
@@ -403,7 +415,7 @@
     <t>fabienne.gasser@edubs.ch</t>
   </si>
   <si>
-    <t>20</t>
+    <t>21</t>
   </si>
   <si>
     <t>Friederike</t>
@@ -418,7 +430,7 @@
     <t>friederike.gaiser@edubs.ch</t>
   </si>
   <si>
-    <t>21</t>
+    <t>22</t>
   </si>
   <si>
     <t>Grgic</t>
@@ -430,7 +442,7 @@
     <t>andrea.grgic@edubs.ch</t>
   </si>
   <si>
-    <t>22</t>
+    <t>23</t>
   </si>
   <si>
     <t>Niels</t>
@@ -445,7 +457,7 @@
     <t>niels.grossen@edubs.ch</t>
   </si>
   <si>
-    <t>23</t>
+    <t>24</t>
   </si>
   <si>
     <t>Gut</t>
@@ -457,7 +469,7 @@
     <t>andreas.gut@edubs.ch</t>
   </si>
   <si>
-    <t>24</t>
+    <t>25</t>
   </si>
   <si>
     <t>Alexandra</t>
@@ -472,7 +484,7 @@
     <t>alexandra.guski@bs.ch</t>
   </si>
   <si>
-    <t>25</t>
+    <t>26</t>
   </si>
   <si>
     <t>Teresa</t>
@@ -487,7 +499,7 @@
     <t>teresa.guarini@edubs.ch</t>
   </si>
   <si>
-    <t>26</t>
+    <t>27</t>
   </si>
   <si>
     <t>Thomas</t>
@@ -502,7 +514,7 @@
     <t>thomas.gysin@edubs.ch</t>
   </si>
   <si>
-    <t>27</t>
+    <t>28</t>
   </si>
   <si>
     <t>Beatris</t>
@@ -517,7 +529,7 @@
     <t>beatris.heinzmann@edubs.ch</t>
   </si>
   <si>
-    <t>28</t>
+    <t>29</t>
   </si>
   <si>
     <t>Markus</t>
@@ -532,7 +544,7 @@
     <t>markus.heinzer@edubs.ch</t>
   </si>
   <si>
-    <t>29</t>
+    <t>30</t>
   </si>
   <si>
     <t>Michael</t>
@@ -547,7 +559,7 @@
     <t>michael.herrmann@edubs.ch</t>
   </si>
   <si>
-    <t>30</t>
+    <t>31</t>
   </si>
   <si>
     <t>Yolanda</t>
@@ -562,7 +574,7 @@
     <t>yolanda.heusser@edubs.ch</t>
   </si>
   <si>
-    <t>31</t>
+    <t>32</t>
   </si>
   <si>
     <t>Sabrina</t>
@@ -577,7 +589,7 @@
     <t>sabrina.hintermann@edubs.ch</t>
   </si>
   <si>
-    <t>32</t>
+    <t>33</t>
   </si>
   <si>
     <t>Stephan</t>
@@ -592,7 +604,7 @@
     <t>stephan.hochkeppel@edubs.ch</t>
   </si>
   <si>
-    <t>33</t>
+    <t>34</t>
   </si>
   <si>
     <t>Salomé</t>
@@ -607,7 +619,7 @@
     <t>salome.huggel@edubs.ch</t>
   </si>
   <si>
-    <t>34</t>
+    <t>35</t>
   </si>
   <si>
     <t>Patrick</t>
@@ -622,7 +634,7 @@
     <t>patrick.jeannotat@edubs.ch</t>
   </si>
   <si>
-    <t>35</t>
+    <t>36</t>
   </si>
   <si>
     <t>Ruedi</t>
@@ -637,7 +649,7 @@
     <t>rjr@jean-richard.ch</t>
   </si>
   <si>
-    <t>36</t>
+    <t>37</t>
   </si>
   <si>
     <t>Werner</t>
@@ -652,7 +664,7 @@
     <t>werner.jenni@edubs.ch</t>
   </si>
   <si>
-    <t>37</t>
+    <t>38</t>
   </si>
   <si>
     <t>Anina</t>
@@ -667,7 +679,7 @@
     <t>anina.jost@edubs.ch</t>
   </si>
   <si>
-    <t>38</t>
+    <t>39</t>
   </si>
   <si>
     <t>Boas</t>
@@ -682,7 +694,7 @@
     <t>boas.kirchhofer@edubs.ch</t>
   </si>
   <si>
-    <t>39</t>
+    <t>40</t>
   </si>
   <si>
     <t>Kläy</t>
@@ -694,7 +706,7 @@
     <t>nicole.klaey@edubs.ch</t>
   </si>
   <si>
-    <t>40</t>
+    <t>41</t>
   </si>
   <si>
     <t>Gabriele</t>
@@ -709,7 +721,7 @@
     <t>gabriele.knuemann@edubs.ch</t>
   </si>
   <si>
-    <t>41</t>
+    <t>42</t>
   </si>
   <si>
     <t>Oliver</t>
@@ -724,7 +736,7 @@
     <t>oliver.kubetzko@edubs.ch</t>
   </si>
   <si>
-    <t>42</t>
+    <t>43</t>
   </si>
   <si>
     <t>Klemens</t>
@@ -739,7 +751,7 @@
     <t>klemens@foolpool.de</t>
   </si>
   <si>
-    <t>43</t>
+    <t>44</t>
   </si>
   <si>
     <t>Stefan</t>
@@ -754,7 +766,7 @@
     <t>stefan_camenzind@sunrise.ch</t>
   </si>
   <si>
-    <t>44</t>
+    <t>45</t>
   </si>
   <si>
     <t>Dominique</t>
@@ -769,7 +781,7 @@
     <t>dominique.luedi@gmail.com</t>
   </si>
   <si>
-    <t>45</t>
+    <t>46</t>
   </si>
   <si>
     <t>Kaspar</t>
@@ -784,7 +796,7 @@
     <t>chluescher@sunrise.ch</t>
   </si>
   <si>
-    <t>46</t>
+    <t>47</t>
   </si>
   <si>
     <t>Tiziana</t>
@@ -799,7 +811,7 @@
     <t>mail@tiziana-sarro.net</t>
   </si>
   <si>
-    <t>47</t>
+    <t>48</t>
   </si>
   <si>
     <t>Fiona</t>
@@ -814,7 +826,7 @@
     <t>fionaschreier@gmail.com</t>
   </si>
   <si>
-    <t>48</t>
+    <t>49</t>
   </si>
   <si>
     <t>Renate</t>
@@ -829,7 +841,7 @@
     <t>renateju@gmx.ch</t>
   </si>
   <si>
-    <t>49</t>
+    <t>50</t>
   </si>
   <si>
     <t>Zgorolec</t>
@@ -841,7 +853,7 @@
     <t>oli.z@gmx.ch</t>
   </si>
   <si>
-    <t>50</t>
+    <t>51</t>
   </si>
   <si>
     <t>Raphael</t>
@@ -856,7 +868,7 @@
     <t>raphael.kuebler@edubs.ch</t>
   </si>
   <si>
-    <t>51</t>
+    <t>52</t>
   </si>
   <si>
     <t>Elena</t>
@@ -871,7 +883,7 @@
     <t>elena.leuenberger@edubs.ch</t>
   </si>
   <si>
-    <t>52</t>
+    <t>53</t>
   </si>
   <si>
     <t>Leiser</t>
@@ -883,7 +895,7 @@
     <t>martin.leiser@edubs.ch</t>
   </si>
   <si>
-    <t>53</t>
+    <t>54</t>
   </si>
   <si>
     <t>Roland</t>
@@ -898,7 +910,7 @@
     <t>roland.leuthardt@edubs.ch</t>
   </si>
   <si>
-    <t>54</t>
+    <t>55</t>
   </si>
   <si>
     <t>Fabian</t>
@@ -913,7 +925,7 @@
     <t>fabian.loew@edubs.ch</t>
   </si>
   <si>
-    <t>55</t>
+    <t>56</t>
   </si>
   <si>
     <t>Mariella</t>
@@ -928,7 +940,7 @@
     <t>mariella.lucrezia@edubs.ch</t>
   </si>
   <si>
-    <t>56</t>
+    <t>57</t>
   </si>
   <si>
     <t>Romano</t>
@@ -943,7 +955,7 @@
     <t>romano.macuglia@edubs.ch</t>
   </si>
   <si>
-    <t>57</t>
+    <t>58</t>
   </si>
   <si>
     <t>Dinesh</t>
@@ -958,7 +970,7 @@
     <t>dinesh.mehta@edubs.ch</t>
   </si>
   <si>
-    <t>58</t>
+    <t>59</t>
   </si>
   <si>
     <t>Meerstetter</t>
@@ -970,7 +982,7 @@
     <t>f.meerstetter@stud.unibas.ch</t>
   </si>
   <si>
-    <t>59</t>
+    <t>60</t>
   </si>
   <si>
     <t>Annette</t>
@@ -985,7 +997,7 @@
     <t>annette.morenz@edubs.ch</t>
   </si>
   <si>
-    <t>60</t>
+    <t>61</t>
   </si>
   <si>
     <t>Mülken</t>
@@ -997,7 +1009,7 @@
     <t>oliver.muelken@edubs.ch</t>
   </si>
   <si>
-    <t>61</t>
+    <t>62</t>
   </si>
   <si>
     <t>Stefano</t>
@@ -1012,7 +1024,7 @@
     <t>stefano.muratore@edubs.ch</t>
   </si>
   <si>
-    <t>62</t>
+    <t>63</t>
   </si>
   <si>
     <t>Natalie</t>
@@ -1027,7 +1039,7 @@
     <t>natalie.nikitine@edubs.ch</t>
   </si>
   <si>
-    <t>63</t>
+    <t>64</t>
   </si>
   <si>
     <t>Miranda</t>
@@ -1042,7 +1054,7 @@
     <t>miranda.oeschger@edubs.ch</t>
   </si>
   <si>
-    <t>64</t>
+    <t>65</t>
   </si>
   <si>
     <t>Marco</t>
@@ -1057,7 +1069,7 @@
     <t>marco.orsini@edubs.ch</t>
   </si>
   <si>
-    <t>65</t>
+    <t>66</t>
   </si>
   <si>
     <t>Simon</t>
@@ -1072,7 +1084,7 @@
     <t>simon.peter@edubs.ch</t>
   </si>
   <si>
-    <t>66</t>
+    <t>67</t>
   </si>
   <si>
     <t>Lukas</t>
@@ -1087,7 +1099,7 @@
     <t>lukas.pfeifer@edubs.ch</t>
   </si>
   <si>
-    <t>67</t>
+    <t>68</t>
   </si>
   <si>
     <t>Bernd</t>
@@ -1102,7 +1114,7 @@
     <t>bernd.piepenbreier@edubs.ch</t>
   </si>
   <si>
-    <t>68</t>
+    <t>69</t>
   </si>
   <si>
     <t>Erik</t>
@@ -1117,7 +1129,7 @@
     <t>erik.pleuler@bs.ch</t>
   </si>
   <si>
-    <t>69</t>
+    <t>70</t>
   </si>
   <si>
     <t>Ines</t>
@@ -1132,7 +1144,7 @@
     <t>ines.place@edubs.ch</t>
   </si>
   <si>
-    <t>70</t>
+    <t>71</t>
   </si>
   <si>
     <t>Michela</t>
@@ -1147,7 +1159,7 @@
     <t>michela.puopolo@edubs.ch</t>
   </si>
   <si>
-    <t>71</t>
+    <t>72</t>
   </si>
   <si>
     <t>Christine</t>
@@ -1162,7 +1174,7 @@
     <t>christine.reinders@edubs.ch</t>
   </si>
   <si>
-    <t>72</t>
+    <t>73</t>
   </si>
   <si>
     <t>Florian</t>
@@ -1177,7 +1189,7 @@
     <t>florian.recher@edubs.ch</t>
   </si>
   <si>
-    <t>73</t>
+    <t>74</t>
   </si>
   <si>
     <t>Nicola</t>
@@ -1192,7 +1204,7 @@
     <t>nicola.renfer@edubs.ch</t>
   </si>
   <si>
-    <t>74</t>
+    <t>75</t>
   </si>
   <si>
     <t>Daniel</t>
@@ -1207,7 +1219,7 @@
     <t>daniel.roth@edubs.ch</t>
   </si>
   <si>
-    <t>75</t>
+    <t>76</t>
   </si>
   <si>
     <t>Kim</t>
@@ -1222,7 +1234,7 @@
     <t>kim.rossel@edubs.ch</t>
   </si>
   <si>
-    <t>76</t>
+    <t>77</t>
   </si>
   <si>
     <t>Susanne</t>
@@ -1237,7 +1249,7 @@
     <t>susanne.rodriguez@edubs.ch</t>
   </si>
   <si>
-    <t>77</t>
+    <t>78</t>
   </si>
   <si>
     <t>Susi</t>
@@ -1252,7 +1264,7 @@
     <t>susi.rueedi@edubs.ch</t>
   </si>
   <si>
-    <t>78</t>
+    <t>79</t>
   </si>
   <si>
     <t>Tanja</t>
@@ -1267,7 +1279,7 @@
     <t>tanja.ruder@edubs.ch</t>
   </si>
   <si>
-    <t>79</t>
+    <t>80</t>
   </si>
   <si>
     <t>Arnold</t>
@@ -1282,7 +1294,7 @@
     <t>arnold.schumacher@edubs.ch</t>
   </si>
   <si>
-    <t>80</t>
+    <t>81</t>
   </si>
   <si>
     <t>Diego</t>
@@ -1297,7 +1309,7 @@
     <t>diego.scheuber@edubs.ch</t>
   </si>
   <si>
-    <t>81</t>
+    <t>82</t>
   </si>
   <si>
     <t>Schmid</t>
@@ -1309,7 +1321,7 @@
     <t>fabian.schmid@edubs.ch</t>
   </si>
   <si>
-    <t>82</t>
+    <t>83</t>
   </si>
   <si>
     <t>Judith</t>
@@ -1324,7 +1336,7 @@
     <t>judith.schnyder@edubs.ch</t>
   </si>
   <si>
-    <t>83</t>
+    <t>84</t>
   </si>
   <si>
     <t>Mandy</t>
@@ -1339,7 +1351,7 @@
     <t>mandy.schiele@edubs.ch</t>
   </si>
   <si>
-    <t>84</t>
+    <t>85</t>
   </si>
   <si>
     <t>Schmidli</t>
@@ -1351,7 +1363,7 @@
     <t>patrick.schmidli@edubs.ch</t>
   </si>
   <si>
-    <t>85</t>
+    <t>86</t>
   </si>
   <si>
     <t>Sieglinde</t>
@@ -1366,7 +1378,7 @@
     <t>sieglinde.schreiner@bs.ch</t>
   </si>
   <si>
-    <t>86</t>
+    <t>87</t>
   </si>
   <si>
     <t>Schmidlin</t>
@@ -1378,7 +1390,7 @@
     <t>thomas.schmidlin@edubs.ch</t>
   </si>
   <si>
-    <t>87</t>
+    <t>88</t>
   </si>
   <si>
     <t>Rachel</t>
@@ -1393,7 +1405,7 @@
     <t>rachel.stucky@edubs.ch</t>
   </si>
   <si>
-    <t>88</t>
+    <t>89</t>
   </si>
   <si>
     <t>Tanja Maria</t>
@@ -1408,7 +1420,7 @@
     <t>tanja.stoller@edubs.ch</t>
   </si>
   <si>
-    <t>89</t>
+    <t>90</t>
   </si>
   <si>
     <t>Michèle-Adeline</t>
@@ -1423,7 +1435,7 @@
     <t>michele.tettue@edubs.ch</t>
   </si>
   <si>
-    <t>90</t>
+    <t>91</t>
   </si>
   <si>
     <t>Beatrice</t>
@@ -1438,7 +1450,7 @@
     <t>beatrice.thiele@edubs.ch</t>
   </si>
   <si>
-    <t>91</t>
+    <t>92</t>
   </si>
   <si>
     <t>Corina</t>
@@ -1453,7 +1465,7 @@
     <t>corina.thommen@edubs.ch</t>
   </si>
   <si>
-    <t>92</t>
+    <t>93</t>
   </si>
   <si>
     <t>Daniela</t>
@@ -1468,7 +1480,7 @@
     <t>daniela.truetsch@edubs.ch</t>
   </si>
   <si>
-    <t>93</t>
+    <t>94</t>
   </si>
   <si>
     <t>Ueli</t>
@@ -1483,7 +1495,7 @@
     <t>ueli.vonarx@edubs.ch</t>
   </si>
   <si>
-    <t>94</t>
+    <t>95</t>
   </si>
   <si>
     <t>Stephanie</t>
@@ -1498,7 +1510,7 @@
     <t>stephanie.buettiker@edubs.ch</t>
   </si>
   <si>
-    <t>95</t>
+    <t>96</t>
   </si>
   <si>
     <t>Angelika</t>
@@ -1513,7 +1525,7 @@
     <t>angelika.wenzel@edubs.ch</t>
   </si>
   <si>
-    <t>96</t>
+    <t>97</t>
   </si>
   <si>
     <t>Anne</t>
@@ -1528,7 +1540,7 @@
     <t>anneweick@gmail.com</t>
   </si>
   <si>
-    <t>97</t>
+    <t>98</t>
   </si>
   <si>
     <t>Monika</t>
@@ -1543,7 +1555,7 @@
     <t>monika.wetli@edubs.ch</t>
   </si>
   <si>
-    <t>98</t>
+    <t>99</t>
   </si>
   <si>
     <t>Corinne</t>
@@ -1558,7 +1570,7 @@
     <t>corinne.wiederkehr@edubs.ch</t>
   </si>
   <si>
-    <t>99</t>
+    <t>100</t>
   </si>
   <si>
     <t>János</t>
@@ -1573,7 +1585,7 @@
     <t>janos.winkler@edubs.ch</t>
   </si>
   <si>
-    <t>100</t>
+    <t>101</t>
   </si>
   <si>
     <t>Sabine</t>
@@ -1588,7 +1600,7 @@
     <t>sabine.wicki1@edubs.ch</t>
   </si>
   <si>
-    <t>101</t>
+    <t>102</t>
   </si>
   <si>
     <t>Wydler</t>
@@ -1600,7 +1612,7 @@
     <t>susanne.wydler@edubs.ch</t>
   </si>
   <si>
-    <t>102</t>
+    <t>103</t>
   </si>
   <si>
     <t>David</t>
@@ -1615,7 +1627,7 @@
     <t>david.zahno@edubs.ch</t>
   </si>
   <si>
-    <t>103</t>
+    <t>104</t>
   </si>
   <si>
     <t>Test</t>
@@ -1630,7 +1642,7 @@
     <t>caa.doz@edubs.ch</t>
   </si>
   <si>
-    <t>104</t>
+    <t>105</t>
   </si>
   <si>
     <t>Doz3</t>
@@ -1642,7 +1654,7 @@
     <t>tos.doz@edubs.ch</t>
   </si>
   <si>
-    <t>105</t>
+    <t>106</t>
   </si>
   <si>
     <t>Doz4</t>
@@ -1654,7 +1666,7 @@
     <t>Haa.doz@edubs.ch</t>
   </si>
   <si>
-    <t>106</t>
+    <t>107</t>
   </si>
   <si>
     <t>Doz5</t>
@@ -1664,73 +1676,131 @@
   </si>
   <si>
     <t>Fcl.doz@edubs.ch</t>
-  </si>
-  <si>
-    <t>107</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
+    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;$&quot;;[Red]\-#,##0.00\ &quot;$&quot;"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;$&quot;_-;\-* #,##0\ &quot;$&quot;_-;_-* &quot;-&quot;\ &quot;$&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0\ _$_-;\-* #,##0\ _$_-;_-* &quot;-&quot;\ _$_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1593875898" ulstyle="none" kern="1">
+            <pm:latin face="Calibri" sz="240" lang="default"/>
+            <pm:cs face="Basic Roman" sz="240" lang="default"/>
+            <pm:ea face="Basic Roman" sz="240" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <name val="Basic Sans"/>
+      <family val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1593875898" ulstyle="none" kern="1">
+            <pm:latin face="Basic Sans" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1593875898" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1593875898"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1593875898"/>
+        </ext>
+      </extLst>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="smNativeData">
+      <pm:charStyles xmlns:pm="smNativeData" id="1593875898" count="1">
+        <pm:charStyle name="Normal" fontId="0" Id="1"/>
+      </pm:charStyles>
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Peer Juettner" id="{11F6CBDB-E852-4C95-9621-6418A4171369}" userId="Peer Juettner" providerId="None"/>
-</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1738,16 +1808,16 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="D5D5D5"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="494949"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="EEECE1"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="1F497D"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="4F81BD"/>
@@ -1779,71 +1849,11 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:ea typeface="Basic Roman"/>
+        <a:cs typeface="Basic Roman"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1878,16 +1888,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -2012,16 +2026,25 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
+      <a:bodyPr>
+        <a:prstTxWarp prst="textNoShape">
+          <a:avLst/>
+        </a:prstTxWarp>
+        <a:noAutofit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr>
+          <a:defRPr/>
+        </a:defPPr>
+      </a:lstStyle>
       <a:style>
-        <a:lnRef idx="1">
+        <a:lnRef idx="0">
           <a:schemeClr val="accent1"/>
         </a:lnRef>
-        <a:fillRef idx="3">
+        <a:fillRef idx="0">
           <a:schemeClr val="accent1"/>
         </a:fillRef>
-        <a:effectRef idx="2">
+        <a:effectRef idx="0">
           <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -2029,61 +2052,22 @@
         </a:fontRef>
       </a:style>
     </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
   </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A1" dT="2020-03-21T13:30:52.16" personId="{11F6CBDB-E852-4C95-9621-6418A4171369}" id="{2A1E609B-5249-4D08-B548-F3C7C60441AC}">
-    <text>Vorname des Dozenten/Experten</text>
-  </threadedComment>
-  <threadedComment ref="B1" dT="2020-03-21T13:31:08.42" personId="{11F6CBDB-E852-4C95-9621-6418A4171369}" id="{0E2F502E-311A-4D81-9115-93705B70C95D}">
-    <text>Nachname des dozenten/experten</text>
-  </threadedComment>
-  <threadedComment ref="C1" dT="2020-03-21T13:31:55.16" personId="{11F6CBDB-E852-4C95-9621-6418A4171369}" id="{511EB7D9-C334-404E-82D3-AF6388B14F2E}">
-    <text>Kürzel des dozenten. Muss mit dem Dozentenkürzel bei den Präsentationen übereinstimmen.</text>
-  </threadedComment>
-  <threadedComment ref="D1" dT="2020-03-21T13:32:43.44" personId="{11F6CBDB-E852-4C95-9621-6418A4171369}" id="{D6A8E29B-FDC6-4920-8EFE-04825474B544}">
-    <text>Email des Dozenten/Experten.</text>
-  </threadedComment>
-  <threadedComment ref="E1" dT="2020-03-21T13:32:25.43" personId="{11F6CBDB-E852-4C95-9621-6418A4171369}" id="{55035905-0A00-4588-99BC-9E1F5B6F3589}">
-    <text>ID des Dozenten/Experten. Muss bei 0 beginnen und aufsteigen. Eine ID darf nicht doppelt vergeben werden.</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.60"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2100,7 +2084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2117,7 +2101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2134,7 +2118,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2151,7 +2135,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2168,7 +2152,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2185,7 +2169,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2202,7 +2186,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2219,7 +2203,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -2236,7 +2220,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2253,7 +2237,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2270,7 +2254,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -2287,7 +2271,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -2304,7 +2288,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -2321,7 +2305,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -2338,7 +2322,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -2355,7 +2339,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -2372,7 +2356,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -2389,7 +2373,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -2406,7 +2390,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>95</v>
       </c>
@@ -2423,7 +2407,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -2440,7 +2424,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -2457,7 +2441,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -2474,12 +2458,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
         <v>116</v>
@@ -2491,7 +2475,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>119</v>
       </c>
@@ -2508,12 +2492,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="B26" t="s">
-        <v>124</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
         <v>125</v>
@@ -2525,7 +2509,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -2542,7 +2526,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -2559,7 +2543,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>138</v>
       </c>
@@ -2576,7 +2560,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -2593,7 +2577,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -2610,7 +2594,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -2627,7 +2611,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>158</v>
       </c>
@@ -2644,7 +2628,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>163</v>
       </c>
@@ -2661,7 +2645,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>168</v>
       </c>
@@ -2678,7 +2662,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>173</v>
       </c>
@@ -2695,7 +2679,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>178</v>
       </c>
@@ -2712,7 +2696,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>183</v>
       </c>
@@ -2729,7 +2713,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>188</v>
       </c>
@@ -2746,7 +2730,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>193</v>
       </c>
@@ -2763,7 +2747,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>198</v>
       </c>
@@ -2780,12 +2764,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>203</v>
       </c>
       <c r="B42" t="s">
-        <v>203</v>
+        <v>26</v>
       </c>
       <c r="C42" t="s">
         <v>204</v>
@@ -2797,7 +2781,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>207</v>
       </c>
@@ -2814,7 +2798,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>212</v>
       </c>
@@ -2831,7 +2815,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>217</v>
       </c>
@@ -2848,7 +2832,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>222</v>
       </c>
@@ -2865,7 +2849,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>227</v>
       </c>
@@ -2882,7 +2866,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>232</v>
       </c>
@@ -2899,7 +2883,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>237</v>
       </c>
@@ -2916,7 +2900,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>242</v>
       </c>
@@ -2933,7 +2917,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -2950,12 +2934,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>212</v>
+        <v>252</v>
       </c>
       <c r="B52" t="s">
-        <v>252</v>
+        <v>213</v>
       </c>
       <c r="C52" t="s">
         <v>253</v>
@@ -2967,7 +2951,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>256</v>
       </c>
@@ -2984,7 +2968,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>261</v>
       </c>
@@ -3001,12 +2985,12 @@
         <v>265</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>266</v>
       </c>
       <c r="B55" t="s">
-        <v>266</v>
+        <v>36</v>
       </c>
       <c r="C55" t="s">
         <v>267</v>
@@ -3018,7 +3002,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>270</v>
       </c>
@@ -3035,7 +3019,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>275</v>
       </c>
@@ -3052,7 +3036,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>280</v>
       </c>
@@ -3069,7 +3053,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>285</v>
       </c>
@@ -3086,7 +3070,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>290</v>
       </c>
@@ -3103,12 +3087,12 @@
         <v>294</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>105</v>
+        <v>295</v>
       </c>
       <c r="B61" t="s">
-        <v>295</v>
+        <v>106</v>
       </c>
       <c r="C61" t="s">
         <v>296</v>
@@ -3120,7 +3104,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>299</v>
       </c>
@@ -3137,12 +3121,12 @@
         <v>303</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>212</v>
+        <v>304</v>
       </c>
       <c r="B63" t="s">
-        <v>304</v>
+        <v>213</v>
       </c>
       <c r="C63" t="s">
         <v>305</v>
@@ -3154,7 +3138,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>308</v>
       </c>
@@ -3171,7 +3155,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>313</v>
       </c>
@@ -3188,7 +3172,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>318</v>
       </c>
@@ -3205,7 +3189,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>323</v>
       </c>
@@ -3222,7 +3206,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>328</v>
       </c>
@@ -3239,7 +3223,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>333</v>
       </c>
@@ -3256,7 +3240,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>338</v>
       </c>
@@ -3273,7 +3257,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>343</v>
       </c>
@@ -3290,7 +3274,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>348</v>
       </c>
@@ -3307,7 +3291,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>353</v>
       </c>
@@ -3324,7 +3308,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>358</v>
       </c>
@@ -3341,7 +3325,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>363</v>
       </c>
@@ -3358,7 +3342,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>368</v>
       </c>
@@ -3375,7 +3359,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>373</v>
       </c>
@@ -3392,7 +3376,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>378</v>
       </c>
@@ -3409,7 +3393,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>383</v>
       </c>
@@ -3426,7 +3410,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>388</v>
       </c>
@@ -3443,7 +3427,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>393</v>
       </c>
@@ -3460,7 +3444,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>398</v>
       </c>
@@ -3477,7 +3461,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>403</v>
       </c>
@@ -3494,12 +3478,12 @@
         <v>407</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>275</v>
+        <v>408</v>
       </c>
       <c r="B84" t="s">
-        <v>408</v>
+        <v>276</v>
       </c>
       <c r="C84" t="s">
         <v>409</v>
@@ -3511,7 +3495,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>412</v>
       </c>
@@ -3528,7 +3512,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>417</v>
       </c>
@@ -3545,12 +3529,12 @@
         <v>421</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>178</v>
+        <v>422</v>
       </c>
       <c r="B87" t="s">
-        <v>422</v>
+        <v>179</v>
       </c>
       <c r="C87" t="s">
         <v>423</v>
@@ -3562,7 +3546,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>426</v>
       </c>
@@ -3579,12 +3563,12 @@
         <v>430</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>138</v>
+        <v>431</v>
       </c>
       <c r="B89" t="s">
-        <v>431</v>
+        <v>139</v>
       </c>
       <c r="C89" t="s">
         <v>432</v>
@@ -3596,7 +3580,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>435</v>
       </c>
@@ -3613,7 +3597,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>440</v>
       </c>
@@ -3630,7 +3614,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>445</v>
       </c>
@@ -3647,7 +3631,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>450</v>
       </c>
@@ -3664,7 +3648,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>455</v>
       </c>
@@ -3681,7 +3665,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>460</v>
       </c>
@@ -3698,7 +3682,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>465</v>
       </c>
@@ -3715,7 +3699,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>470</v>
       </c>
@@ -3732,7 +3716,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>475</v>
       </c>
@@ -3749,7 +3733,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>480</v>
       </c>
@@ -3766,7 +3750,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>485</v>
       </c>
@@ -3783,7 +3767,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>490</v>
       </c>
@@ -3800,7 +3784,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>495</v>
       </c>
@@ -3817,7 +3801,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>500</v>
       </c>
@@ -3834,12 +3818,12 @@
         <v>504</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>383</v>
+        <v>505</v>
       </c>
       <c r="B104" t="s">
-        <v>505</v>
+        <v>384</v>
       </c>
       <c r="C104" t="s">
         <v>506</v>
@@ -3851,7 +3835,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
         <v>509</v>
       </c>
@@ -3868,7 +3852,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
         <v>514</v>
       </c>
@@ -3885,12 +3869,12 @@
         <v>518</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="B107" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C107" t="s">
         <v>520</v>
@@ -3902,12 +3886,12 @@
         <v>522</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>514</v>
+        <v>523</v>
       </c>
       <c r="B108" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="C108" t="s">
         <v>524</v>
@@ -3919,12 +3903,12 @@
         <v>526</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>514</v>
+        <v>527</v>
       </c>
       <c r="B109" t="s">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="C109" t="s">
         <v>528</v>
@@ -3937,10 +3921,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:F111" numberStoredAsText="1"/>
-  </ignoredErrors>
-  <legacyDrawing r:id="rId1"/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1593875898" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.300000" footer="0.300000"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1593875898" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1593875898" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1593875898" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>